<commit_message>
Cambios menores enn plantillas y actualización 2024: falta revisar plantilla beamer
</commit_message>
<xml_diff>
--- a/inst/templates/presupuesto.xlsx
+++ b/inst/templates/presupuesto.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">46010 Valencia</t>
   </si>
   <si>
-    <t xml:space="preserve">N.º PRESUPUESTO: SE23XXX</t>
+    <t xml:space="preserve">N.º PRESUPUESTO: SE24XXX</t>
   </si>
   <si>
     <t xml:space="preserve">Facturar a: XXXXXX</t>
@@ -86,14 +86,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -149,14 +148,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -290,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,7 +299,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -319,11 +314,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,31 +327,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -371,20 +338,24 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -392,15 +363,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -408,39 +379,43 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -448,35 +423,27 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -484,7 +451,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -570,9 +537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1237680</xdr:colOff>
+      <xdr:colOff>1237320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -586,7 +553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4335840" y="107280"/>
-          <a:ext cx="4799880" cy="784440"/>
+          <a:ext cx="4799520" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,6 +568,112 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -608,8 +681,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -638,28 +711,28 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -667,7 +740,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="str">
         <f aca="true">CONCATENATE("FECHA: ",TEXT(TODAY(),"dd/mm/yyyy"))</f>
-        <v>FECHA: 02/01/2023</v>
+        <v>FECHA: 28/05/2024</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
@@ -687,82 +760,82 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25" t="n">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="25" t="n">
+      <c r="D16" s="20" t="n">
         <v>37</v>
       </c>
-      <c r="E16" s="26" t="n">
+      <c r="E16" s="21" t="n">
         <f aca="false">D16*C16</f>
         <v>0</v>
       </c>
@@ -771,198 +844,194 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" s="2" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25" t="n">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="25" t="n">
+      <c r="D18" s="20" t="n">
         <v>37</v>
       </c>
-      <c r="E18" s="26" t="n">
+      <c r="E18" s="21" t="n">
         <f aca="false">D18*C18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" s="2" customFormat="true" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="25" t="n">
+      <c r="B20" s="23"/>
+      <c r="C20" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="25" t="n">
+      <c r="D20" s="20" t="n">
         <v>37</v>
       </c>
-      <c r="E20" s="26" t="n">
+      <c r="E20" s="21" t="n">
         <f aca="false">D20*C20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
+    <row r="21" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="31" t="n">
+      <c r="B22" s="12"/>
+      <c r="C22" s="26" t="n">
         <f aca="false">SUM(C15:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="32" t="n">
+      <c r="E22" s="28" t="n">
         <f aca="false">+SUM(E16:E21)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="0"/>
-      <c r="G22" s="0"/>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="29"/>
+      <c r="C23" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="35" t="n">
+      <c r="D23" s="30"/>
+      <c r="E23" s="31" t="n">
         <f aca="false">E22</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="36" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="37" t="str">
+      <c r="D24" s="32"/>
+      <c r="E24" s="33" t="str">
         <f aca="false">+CONCATENATE(E23," *")</f>
         <v>0 *</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="38" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="45"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="37"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="42"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="25">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E5"/>
     <mergeCell ref="A2:B2"/>
@@ -973,12 +1042,7 @@
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A8:E13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:B18"/>
@@ -988,11 +1052,7 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A27:E31"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A35:E35"/>

</xml_diff>

<commit_message>
Actualizar fechas y logos; eliminar nci
</commit_message>
<xml_diff>
--- a/inst/templates/presupuesto.xlsx
+++ b/inst/templates/presupuesto.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">46010 Valencia</t>
   </si>
   <si>
-    <t xml:space="preserve">N.º PRESUPUESTO: SE25XXX</t>
+    <t xml:space="preserve">N.º PRESUPUESTO: SE26XXX</t>
   </si>
   <si>
     <t xml:space="preserve">Facturar a: XXXXXX</t>
@@ -43,8 +43,26 @@
     <t xml:space="preserve">Enviar a: XXXXXXXX</t>
   </si>
   <si>
-    <t xml:space="preserve">REVISAR POR PROYECTO
-Se aplica un 20 % de descuento sobre la tarifa por hora habitual, al tratarse de personal vinculado a Fisabio (29.6 €/hora en lugar de 37 €/hora).</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">REVISAR POR PROYECTO
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Se aplica la Tarifa A, al tratarse de personal vinculado a Fisabio.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPCIÓN</t>
@@ -96,7 +114,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,6 +151,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -285,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,6 +358,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,7 +454,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,15 +466,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,9 +569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1236960</xdr:colOff>
+      <xdr:colOff>1236600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -556,8 +584,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4336560" y="139320"/>
-          <a:ext cx="4798440" cy="719640"/>
+          <a:off x="3833640" y="139320"/>
+          <a:ext cx="4361400" cy="719280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -686,10 +714,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.43"/>
@@ -744,7 +772,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="str">
         <f aca="true">CONCATENATE("FECHA: ",TEXT(TODAY(),"dd/mm/yyyy"))</f>
-        <v>FECHA: 13/01/2025</v>
+        <v>FECHA: 19/02/2026</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
@@ -786,6 +814,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
@@ -809,39 +838,39 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="n">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="20" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="E16" s="21" t="n">
+      <c r="D16" s="21" t="n">
+        <v>37.93</v>
+      </c>
+      <c r="E16" s="22" t="n">
         <f aca="false">D16*C16</f>
         <v>0</v>
       </c>
@@ -852,187 +881,187 @@
     </row>
     <row r="17" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18" s="2" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20" t="n">
+      <c r="B18" s="20"/>
+      <c r="C18" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="20" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="E18" s="21" t="n">
+      <c r="D18" s="21" t="n">
+        <v>37.93</v>
+      </c>
+      <c r="E18" s="22" t="n">
         <f aca="false">D18*C18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" s="2" customFormat="true" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="24"/>
+      <c r="C20" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="20" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="E20" s="21" t="n">
+      <c r="D20" s="21" t="n">
+        <v>37.93</v>
+      </c>
+      <c r="E20" s="22" t="n">
         <f aca="false">D20*C20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="26" t="n">
+      <c r="B22" s="13"/>
+      <c r="C22" s="27" t="n">
         <f aca="false">SUM(C15:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="28" t="n">
+      <c r="E22" s="29" t="n">
         <f aca="false">+SUM(E16:E21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31" t="n">
+      <c r="D23" s="31"/>
+      <c r="E23" s="32" t="n">
         <f aca="false">E22</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="32" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33" t="str">
+      <c r="D24" s="33"/>
+      <c r="E24" s="34" t="str">
         <f aca="false">+CONCATENATE(E23," *")</f>
         <v>0 *</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="34" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="37"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="38"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1062,6 +1091,9 @@
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" display="Tarifa A"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1069,6 +1101,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>